<commit_message>
PROS-7069 BIPH Template Changes
</commit_message>
<xml_diff>
--- a/Projects/BIPH/Data/Template.xlsx
+++ b/Projects/BIPH/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -866,7 +866,7 @@
     <numFmt numFmtId="166" formatCode="0.00"/>
     <numFmt numFmtId="167" formatCode="0"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -888,13 +888,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -951,21 +944,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1009,11 +991,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -1111,7 +1088,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1224,15 +1201,8 @@
       <bottom style="medium"/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1256,25 +1226,21 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1326,131 +1292,131 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="4" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="17" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1462,67 +1428,51 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="6" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="13" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="13" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="14" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="14" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="15" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="15" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="22" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1530,132 +1480,111 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="8" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="20" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="24" fillId="8" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="false" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="2" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="10" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="11" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="12" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="12" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Normal 2" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1733,13 +1662,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.0647773279352"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -2003,15 +1932,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.2105263157895"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="13" width="17.8906882591093"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="19.4008097165992"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="13" width="18.1012145748988"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="19.7085020242915"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2607,11 +2536,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.1740890688259"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.0647773279352"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.2105263157895"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.246963562753"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="13" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="31.5991902834008"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="21.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2807,15 +2736,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="47" width="20.7813765182186"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="43.17004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="47" width="44.6477732793522"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="47" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="43.919028340081"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="47" width="45.417004048583"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="47" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="47" width="14.8906882591093"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="48" width="15.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="48" width="15.7125506072875"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="48" width="20.8097165991903"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="48" width="24.1174089068826"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="47" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="48" width="15.7449392712551"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="48" width="15.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="48" width="20.995951417004"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="48" width="24.5303643724696"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="48" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2984,10 +2913,10 @@
       <c r="C6" s="54" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="58" t="s">
+      <c r="D6" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="E6" s="59" t="s">
+      <c r="E6" s="56" t="s">
         <v>76</v>
       </c>
       <c r="F6" s="57" t="n">
@@ -3048,22 +2977,22 @@
       <c r="A8" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="60" t="s">
+      <c r="B8" s="58" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="60" t="s">
+      <c r="C8" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="47" t="s">
         <v>65</v>
       </c>
-      <c r="E8" s="62" t="n">
+      <c r="E8" s="58" t="n">
         <v>4800136730057</v>
       </c>
-      <c r="F8" s="60" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="60" t="n">
+      <c r="F8" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="58" t="n">
         <v>1</v>
       </c>
       <c r="H8" s="47" t="n">
@@ -3083,22 +3012,22 @@
       <c r="A9" s="53" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="58" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="62" t="s">
+      <c r="D9" s="58" t="s">
         <v>78</v>
       </c>
-      <c r="E9" s="62" t="n">
+      <c r="E9" s="58" t="n">
         <v>4800136060062</v>
       </c>
-      <c r="F9" s="60" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="60" t="n">
+      <c r="F9" s="58" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="58" t="n">
         <v>1</v>
       </c>
       <c r="H9" s="47" t="n">
@@ -3115,13 +3044,13 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="64"/>
-      <c r="F10" s="64"/>
-      <c r="G10" s="64"/>
+      <c r="A10" s="59"/>
+      <c r="B10" s="60"/>
+      <c r="C10" s="60"/>
+      <c r="D10" s="60"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="60"/>
+      <c r="G10" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3145,21 +3074,21 @@
   </sheetPr>
   <dimension ref="A1:K32"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="65" width="32.3481781376518"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="65" width="26.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="65" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.5303643724696"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="28.9230769230769"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="61" width="32.7773279352227"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.4939271255061"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="61" width="26.7813765182186"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="61" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="13" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="13" width="18.1012145748988"/>
     <col collapsed="false" hidden="false" max="10" min="8" style="14" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="24.251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="24.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -3179,19 +3108,19 @@
       <c r="K1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="87.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="66" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="66" t="s">
+      <c r="A2" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="62" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="66" t="s">
+      <c r="C2" s="62" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="66" t="s">
+      <c r="D2" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="66" t="s">
+      <c r="E2" s="62" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
@@ -3214,560 +3143,560 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="64" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="D3" s="69" t="s">
+      <c r="D3" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="70" t="s">
+      <c r="E3" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="71" t="n">
+      <c r="F3" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="64" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="68" t="s">
+      <c r="C4" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="71" t="n">
+      <c r="F4" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="67" t="s">
+      <c r="A5" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="64" t="s">
         <v>83</v>
       </c>
-      <c r="C5" s="68" t="s">
+      <c r="C5" s="65" t="s">
         <v>84</v>
       </c>
-      <c r="D5" s="69" t="s">
+      <c r="D5" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="70" t="s">
+      <c r="E5" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F5" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="71" t="n">
+      <c r="F5" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="67" t="s">
+      <c r="A6" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="33" t="s">
+      <c r="B6" s="64" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="68" t="s">
+      <c r="C6" s="65" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="70" t="s">
+      <c r="D6" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="70" t="s">
+      <c r="E6" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="71" t="n">
+      <c r="F6" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="73" t="s">
+      <c r="A7" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="72" t="s">
+      <c r="B7" s="69" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="E7" s="75" t="s">
+      <c r="E7" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="71" t="n">
+      <c r="F7" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="73" t="s">
+      <c r="A8" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="72" t="s">
+      <c r="B8" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="71" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="75" t="s">
+      <c r="E8" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="71" t="n">
+      <c r="F8" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="65" t="s">
         <v>92</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="70" t="s">
+      <c r="E9" s="67" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J9" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" s="71" t="n">
+      <c r="F9" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J9" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="68" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="33" t="s">
+      <c r="B10" s="64" t="s">
         <v>93</v>
       </c>
-      <c r="C10" s="68" t="s">
+      <c r="C10" s="65" t="s">
         <v>94</v>
       </c>
-      <c r="D10" s="70" t="s">
+      <c r="D10" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="E10" s="70" t="s">
+      <c r="E10" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="71" t="n">
+      <c r="F10" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="68" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="67" t="s">
+      <c r="A11" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="33" t="s">
+      <c r="B11" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="D11" s="69" t="s">
+      <c r="D11" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="70" t="s">
+      <c r="E11" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="71" t="n">
+      <c r="F11" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="65" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="67" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="68" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="67" t="s">
+      <c r="A12" s="63" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="33" t="s">
+      <c r="B12" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="C12" s="68" t="s">
+      <c r="C12" s="65" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="E12" s="70" t="s">
+      <c r="E12" s="67" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="71" t="n">
+      <c r="F12" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="73" t="s">
+      <c r="A13" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="72" t="s">
+      <c r="B13" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="71" t="s">
         <v>100</v>
       </c>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="72" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="75" t="s">
+      <c r="E13" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F13" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J13" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="K13" s="76" t="n">
+      <c r="F13" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="I13" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J13" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="K13" s="68" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="73" t="s">
+      <c r="A14" s="70" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="72" t="s">
+      <c r="B14" s="69" t="s">
         <v>101</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="E14" s="75" t="s">
+      <c r="E14" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="72" t="n">
-        <v>0</v>
-      </c>
-      <c r="G14" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="H14" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="72" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="76" t="n">
+      <c r="F14" s="69" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="J14" s="69" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="68" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="77" t="s">
+      <c r="A15" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="33" t="s">
+      <c r="B15" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="C15" s="68" t="s">
+      <c r="C15" s="65" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="70" t="s">
+      <c r="E15" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F15" s="33" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="I15" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="33" t="n">
-        <v>0</v>
-      </c>
-      <c r="K15" s="78" t="n">
+      <c r="F15" s="64" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="65" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="64" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" s="71" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F16" s="33"/>
-      <c r="H16" s="79"/>
-      <c r="I16" s="70"/>
+      <c r="H16" s="74"/>
+      <c r="I16" s="75"/>
       <c r="J16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F17" s="33"/>
-      <c r="H17" s="79"/>
-      <c r="I17" s="70"/>
+      <c r="H17" s="74"/>
+      <c r="I17" s="75"/>
       <c r="J17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F18" s="33"/>
-      <c r="H18" s="70"/>
-      <c r="I18" s="70"/>
+      <c r="H18" s="75"/>
+      <c r="I18" s="75"/>
       <c r="J18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F19" s="33"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
+      <c r="H19" s="75"/>
+      <c r="I19" s="75"/>
       <c r="J19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F20" s="33"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
+      <c r="H20" s="75"/>
+      <c r="I20" s="75"/>
       <c r="J20" s="33"/>
     </row>
     <row r="21" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F21" s="33"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="70"/>
+      <c r="H21" s="75"/>
+      <c r="I21" s="75"/>
       <c r="J21" s="33"/>
     </row>
     <row r="22" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F22" s="33"/>
-      <c r="H22" s="70"/>
-      <c r="I22" s="70"/>
+      <c r="H22" s="75"/>
+      <c r="I22" s="75"/>
       <c r="J22" s="33"/>
     </row>
     <row r="23" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F23" s="33"/>
-      <c r="H23" s="70"/>
-      <c r="I23" s="70"/>
+      <c r="H23" s="75"/>
+      <c r="I23" s="75"/>
       <c r="J23" s="33"/>
     </row>
     <row r="24" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F24" s="33"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
+      <c r="H24" s="75"/>
+      <c r="I24" s="75"/>
       <c r="J24" s="33"/>
     </row>
     <row r="25" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33"/>
-      <c r="H25" s="70"/>
-      <c r="I25" s="70"/>
+      <c r="H25" s="75"/>
+      <c r="I25" s="75"/>
       <c r="J25" s="33"/>
     </row>
     <row r="26" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="33"/>
-      <c r="H26" s="70"/>
-      <c r="I26" s="70"/>
+      <c r="H26" s="75"/>
+      <c r="I26" s="75"/>
       <c r="J26" s="33"/>
     </row>
     <row r="27" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33"/>
-      <c r="H27" s="70"/>
-      <c r="I27" s="70"/>
+      <c r="H27" s="75"/>
+      <c r="I27" s="75"/>
       <c r="J27" s="33"/>
     </row>
     <row r="28" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="33"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
+      <c r="H28" s="75"/>
+      <c r="I28" s="75"/>
       <c r="J28" s="33"/>
     </row>
     <row r="29" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F29" s="33"/>
-      <c r="H29" s="70"/>
-      <c r="I29" s="70"/>
+      <c r="H29" s="75"/>
+      <c r="I29" s="75"/>
       <c r="J29" s="33"/>
     </row>
     <row r="30" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="33"/>
-      <c r="H30" s="70"/>
-      <c r="I30" s="70"/>
+      <c r="H30" s="75"/>
+      <c r="I30" s="75"/>
       <c r="J30" s="33"/>
     </row>
     <row r="31" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="33"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="70"/>
+      <c r="H31" s="74"/>
+      <c r="I31" s="75"/>
       <c r="J31" s="33"/>
     </row>
     <row r="32" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="33"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="70"/>
+      <c r="H32" s="74"/>
+      <c r="I32" s="75"/>
       <c r="J32" s="33"/>
     </row>
   </sheetData>
@@ -3790,21 +3719,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:K65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J24" activeCellId="0" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="42.9554655870445"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.4615384615385"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="31.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="43.7044534412956"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.6761133603239"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="13" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="14" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="13" width="18.2105263157895"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="14" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="24.9433198380567"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="14" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3823,375 +3754,1776 @@
       <c r="K1" s="16"/>
     </row>
     <row r="2" customFormat="false" ht="87.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="80" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="80" t="s">
+      <c r="A2" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="76" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="80" t="s">
+      <c r="C2" s="76" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="80" t="s">
+      <c r="D2" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="80" t="s">
+      <c r="E2" s="76" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="81" t="s">
+      <c r="F2" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="81" t="s">
+      <c r="G2" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="81" t="s">
+      <c r="H2" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="81" t="s">
+      <c r="I2" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="81" t="s">
+      <c r="J2" s="77" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="81" t="s">
+      <c r="K2" s="77" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="82" t="s">
+      <c r="A3" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="83" t="s">
+      <c r="B3" s="78" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="84" t="n">
+      <c r="C3" s="79" t="n">
         <v>4800136730057</v>
       </c>
-      <c r="D3" s="85" t="s">
+      <c r="D3" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="85" t="s">
+      <c r="E3" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="F3" s="86" t="n">
+      <c r="F3" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="86" t="n">
+      <c r="G3" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="I3" s="86" t="n">
+      <c r="I3" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="J3" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="87" t="n">
+      <c r="J3" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="88" t="s">
+      <c r="B4" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="89" t="n">
+      <c r="C4" s="81" t="n">
         <v>4800136060062</v>
       </c>
-      <c r="D4" s="85" t="s">
+      <c r="D4" s="70" t="s">
         <v>53</v>
       </c>
-      <c r="E4" s="85" t="s">
+      <c r="E4" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="86" t="n">
+      <c r="F4" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="G4" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="86" t="n">
+      <c r="G4" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="I4" s="86" t="n">
+      <c r="I4" s="72" t="n">
         <v>2</v>
       </c>
-      <c r="J4" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="87" t="n">
+      <c r="J4" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="86" t="s">
+      <c r="B5" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="90" t="n">
+      <c r="C5" s="82" t="n">
         <v>4800292124547</v>
       </c>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="E5" s="86" t="s">
+      <c r="E5" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="87" t="n">
+      <c r="F5" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="86" t="s">
+      <c r="B6" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="90" t="n">
+      <c r="C6" s="82" t="n">
         <v>4800292408166</v>
       </c>
-      <c r="D6" s="86" t="s">
+      <c r="D6" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="86" t="s">
+      <c r="E6" s="72" t="s">
         <v>62</v>
       </c>
-      <c r="F6" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="86" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="87" t="n">
+      <c r="F6" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="K6" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="91" t="s">
+      <c r="A7" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="92" t="s">
+      <c r="B7" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="93" t="n">
+      <c r="C7" s="84" t="n">
         <v>4800292315013</v>
       </c>
-      <c r="D7" s="92" t="s">
+      <c r="D7" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="92" t="s">
+      <c r="E7" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="92" t="n">
+      <c r="F7" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="94" t="n">
+      <c r="G7" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="85" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="91" t="s">
+      <c r="A8" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="67" t="s">
         <v>57</v>
       </c>
-      <c r="C8" s="93" t="n">
+      <c r="C8" s="84" t="n">
         <v>4800292315037</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="92" t="s">
+      <c r="E8" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="92" t="n">
+      <c r="F8" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" s="94" t="n">
+      <c r="G8" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H8" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K8" s="85" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="91" t="s">
+      <c r="A9" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="92" t="s">
+      <c r="B9" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="93" t="n">
+      <c r="C9" s="84" t="n">
         <v>4800292315129</v>
       </c>
-      <c r="D9" s="92" t="s">
+      <c r="D9" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="92" t="s">
+      <c r="E9" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="92" t="n">
+      <c r="F9" s="67" t="n">
         <v>2</v>
       </c>
-      <c r="G9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="92" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="94" t="n">
+      <c r="G9" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="67" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="85" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="91" t="s">
+      <c r="A10" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="94"/>
-      <c r="C10" s="94"/>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="92"/>
-      <c r="G10" s="92"/>
-      <c r="H10" s="92"/>
-      <c r="I10" s="92"/>
-      <c r="J10" s="92"/>
-      <c r="K10" s="94"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="85"/>
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="67"/>
+      <c r="G10" s="67"/>
+      <c r="H10" s="67"/>
+      <c r="I10" s="67"/>
+      <c r="J10" s="67"/>
+      <c r="K10" s="85"/>
     </row>
     <row r="11" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="94"/>
-      <c r="C11" s="94"/>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="92"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="92"/>
-      <c r="I11" s="92"/>
-      <c r="J11" s="92"/>
-      <c r="K11" s="94"/>
+      <c r="B11" s="85"/>
+      <c r="C11" s="85"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="67"/>
+      <c r="G11" s="67"/>
+      <c r="H11" s="67"/>
+      <c r="I11" s="67"/>
+      <c r="J11" s="67"/>
+      <c r="K11" s="85"/>
     </row>
     <row r="12" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="91" t="s">
+      <c r="A12" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="94"/>
-      <c r="C12" s="94"/>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="92"/>
-      <c r="G12" s="92"/>
-      <c r="H12" s="92"/>
-      <c r="I12" s="92"/>
-      <c r="J12" s="92"/>
-      <c r="K12" s="94"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="85"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="67"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="67"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="85"/>
     </row>
     <row r="13" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="91" t="s">
+      <c r="A13" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="94"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="94"/>
-      <c r="E13" s="94"/>
-      <c r="F13" s="92"/>
-      <c r="G13" s="92"/>
-      <c r="H13" s="92"/>
-      <c r="I13" s="92"/>
-      <c r="J13" s="92"/>
-      <c r="K13" s="94"/>
+      <c r="B13" s="85"/>
+      <c r="C13" s="85"/>
+      <c r="D13" s="85"/>
+      <c r="E13" s="85"/>
+      <c r="F13" s="67"/>
+      <c r="G13" s="67"/>
+      <c r="H13" s="67"/>
+      <c r="I13" s="67"/>
+      <c r="J13" s="67"/>
+      <c r="K13" s="85"/>
     </row>
     <row r="14" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="91" t="s">
+      <c r="A14" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="94"/>
-      <c r="C14" s="94"/>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="92"/>
-      <c r="I14" s="92"/>
-      <c r="J14" s="92"/>
-      <c r="K14" s="94"/>
+      <c r="B14" s="85"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="67"/>
+      <c r="I14" s="67"/>
+      <c r="J14" s="67"/>
+      <c r="K14" s="85"/>
     </row>
     <row r="15" customFormat="false" ht="14.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="91" t="s">
+      <c r="A15" s="83" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="94"/>
-      <c r="C15" s="94"/>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="92"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="92"/>
-      <c r="I15" s="92"/>
-      <c r="J15" s="92"/>
-      <c r="K15" s="94"/>
-    </row>
+      <c r="B15" s="85"/>
+      <c r="C15" s="85"/>
+      <c r="D15" s="85"/>
+      <c r="E15" s="85"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="67"/>
+      <c r="H15" s="67"/>
+      <c r="I15" s="67"/>
+      <c r="J15" s="67"/>
+      <c r="K15" s="85"/>
+    </row>
+    <row r="1047176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047577" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047578" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047579" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047580" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047581" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047582" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047583" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047584" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047585" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047586" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047587" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047588" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047589" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047590" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047591" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047592" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047593" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047594" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047595" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047596" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047597" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047598" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047599" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047600" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047601" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047602" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047603" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047604" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047605" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047606" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047607" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047608" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047609" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047610" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047611" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047612" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047613" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047614" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047615" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047616" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047617" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047618" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047619" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047620" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047621" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047622" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047623" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047624" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047625" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047626" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047627" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047628" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047629" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047630" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047631" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047632" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047633" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047634" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047635" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047636" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047637" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047638" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047639" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047640" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047641" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047642" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047643" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047644" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047645" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047646" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047647" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047648" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047649" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047650" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047651" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047652" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047653" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047654" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047655" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047656" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047657" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047658" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047659" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047660" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047661" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047662" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047663" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047664" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047665" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047666" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047667" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047668" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047669" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047670" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047671" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047672" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047673" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047674" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047675" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047676" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047677" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047678" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047679" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047680" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047681" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047682" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047683" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047684" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047685" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047686" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047687" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047688" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047689" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047690" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047691" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047692" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047693" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047694" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047695" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047696" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047697" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047698" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047699" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047700" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047701" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047702" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047703" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047704" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047705" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047706" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047707" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047708" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047709" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047710" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047711" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047712" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047713" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047714" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047715" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047716" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047717" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047718" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047719" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047720" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047721" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047722" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047723" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047724" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047725" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047726" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047727" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047728" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047729" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047730" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047731" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047732" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047733" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047734" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047735" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047736" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047737" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047738" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047739" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047740" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047741" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047742" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047743" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047744" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047745" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047746" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047747" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047748" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047749" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047750" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047751" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047752" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047753" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047754" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047755" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047756" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047757" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047758" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047759" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047760" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047761" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047762" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047763" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047764" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047765" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047766" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047767" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047768" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047769" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047770" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047771" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047772" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047773" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047774" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047775" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047776" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047777" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047778" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047779" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047780" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047781" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047782" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047783" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047784" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047785" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047786" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047787" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047788" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047789" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047790" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047791" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047792" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047793" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047794" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047795" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047796" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047797" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047798" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047799" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047800" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047801" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047802" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047803" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047804" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047805" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047806" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047807" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047808" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047809" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047810" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047811" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047812" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047813" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047814" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047815" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047816" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047817" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047818" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047819" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047820" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047821" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047822" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047823" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047824" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047825" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047826" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047827" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047828" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047829" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047830" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047831" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047832" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047833" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047834" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047835" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047836" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047837" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047838" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047839" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047840" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047841" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047842" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047843" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047844" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047845" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047846" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047847" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047848" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047849" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047850" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047851" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047852" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047853" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047854" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047855" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047856" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047857" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047858" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047859" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047860" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047861" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047862" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047863" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047864" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047865" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047866" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047867" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047868" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047869" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047870" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047871" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047872" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047873" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047874" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047875" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047876" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047877" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047878" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047879" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047880" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047881" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047882" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047883" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047884" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047885" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047886" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047887" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047888" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047889" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047890" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047891" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047892" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047893" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047894" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047895" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047896" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047897" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047898" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047899" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047900" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047901" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047902" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047903" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047904" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047905" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047906" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047907" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047908" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047909" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047910" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047927" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047928" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047929" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047930" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047931" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047932" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047933" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047934" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047935" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047936" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047937" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047938" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047939" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047940" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047941" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047942" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047943" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047944" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047945" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047946" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047947" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047948" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047949" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047950" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047951" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047952" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047953" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047954" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047955" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047956" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047957" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047958" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047959" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047960" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047961" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047962" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047963" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047964" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047965" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047966" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047967" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047968" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047969" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047970" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047971" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047972" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047973" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047974" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047975" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047976" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047977" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047978" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047979" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047980" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047981" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047982" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047983" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047984" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047985" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047986" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047987" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047988" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047989" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047990" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047991" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047992" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047993" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047994" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047995" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047996" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047997" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047998" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1047999" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048000" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048001" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048002" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048003" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048004" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048005" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048006" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048007" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048008" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048009" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048010" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048011" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048012" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048013" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048014" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048017" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048018" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048019" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048020" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048021" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048022" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048023" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048024" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048025" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048026" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048027" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048028" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048029" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048030" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048031" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048032" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048033" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048034" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048035" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048036" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048037" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048038" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048039" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048040" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048041" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048042" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048043" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048044" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048045" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048046" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048047" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048048" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048049" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048050" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048051" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048052" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048053" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048054" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048055" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048056" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048057" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048058" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048059" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048060" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048061" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048062" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048063" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048064" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048065" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048066" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048067" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048068" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048069" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048070" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048071" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048072" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048073" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048074" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048077" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048078" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048079" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048080" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048081" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048082" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048083" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048084" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048085" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048086" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048087" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048088" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048089" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048090" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048091" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048092" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048093" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048094" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048095" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048096" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048097" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048098" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048099" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048193" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048194" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048195" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048196" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048197" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048198" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048199" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048200" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048201" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048204" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048206" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048207" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048208" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048209" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048210" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048211" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048212" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048213" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048214" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048215" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048216" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048217" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048218" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048219" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048220" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048221" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048222" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048223" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048224" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:K1"/>

</xml_diff>